<commit_message>
Se crea la mayoria de la parte de la ventana de deudas y de abono, ademas se agrega una nueva tabla a la base de datos (productoDeuda)
</commit_message>
<xml_diff>
--- a/ModeloRelacional.xlsx
+++ b/ModeloRelacional.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge Hernandez\Desktop\ventaPHR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F7499FC-510C-4B68-A0F0-B90AAEFCBECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B936D10-F1C3-4AC9-84CE-1FEE0AFCAD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{DA44F68E-5DB1-4386-A0D9-E50E13830AC0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>Usuario</t>
   </si>
@@ -129,6 +129,24 @@
   </si>
   <si>
     <t>total+iva</t>
+  </si>
+  <si>
+    <t>ProductoDeuda</t>
+  </si>
+  <si>
+    <t>precio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pepsi </t>
+  </si>
+  <si>
+    <t>gansito</t>
+  </si>
+  <si>
+    <t>desodorante</t>
+  </si>
+  <si>
+    <t>30_julio_2022</t>
   </si>
 </sst>
 </file>
@@ -219,6 +237,18 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -228,18 +258,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,33 +572,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B0752BE-1B5E-41D3-9664-DCFE9066D5F7}">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-      <c r="E1" s="2" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="10"/>
+      <c r="E1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="4"/>
-      <c r="L1" s="2" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="10"/>
+      <c r="L1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="4"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="10"/>
       <c r="P1" t="s">
         <v>25</v>
       </c>
@@ -643,7 +661,7 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="2">
         <v>44749</v>
       </c>
       <c r="H3" s="1"/>
@@ -667,7 +685,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G4" s="9"/>
+      <c r="G4" s="3"/>
       <c r="P4">
         <v>1</v>
       </c>
@@ -679,7 +697,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G5" s="9"/>
+      <c r="G5" s="3"/>
       <c r="P5">
         <v>1</v>
       </c>
@@ -691,12 +709,12 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -705,13 +723,13 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="4"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="10"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -795,16 +813,16 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="4"/>
-      <c r="Q15" s="2" t="s">
+      <c r="I15" s="9"/>
+      <c r="J15" s="10"/>
+      <c r="Q15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="R15" s="3"/>
-      <c r="S15" s="4"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="10"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -817,9 +835,7 @@
       <c r="D16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="H16" s="1" t="s">
         <v>16</v>
       </c>
@@ -829,7 +845,7 @@
       <c r="J16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="K16" s="4" t="s">
         <v>31</v>
       </c>
       <c r="Q16" s="1" t="s">
@@ -853,9 +869,7 @@
       <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="H17" s="1">
         <v>1</v>
       </c>
@@ -885,9 +899,6 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
       <c r="H18">
         <v>2</v>
       </c>
@@ -905,6 +916,115 @@
       </c>
       <c r="S18">
         <v>3315359998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>